<commit_message>
- Added normalized gini impurity to the state class. This provides insight to the distribution of the labels at a given state. - Enabled label reset based on the gini impurity value at a given state.
</commit_message>
<xml_diff>
--- a/DataAndResults.xlsx
+++ b/DataAndResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Desktop\RLDT_v3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\Source\Repos\Reinforcement-Learning-Based-Decision-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84591126-F8AB-4EFC-B976-F142ABE02A32}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84386A33-A065-404A-9651-AEFF6865B111}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17513" windowHeight="6413" activeTab="2" xr2:uid="{6315DFC8-D662-4E0F-B86A-A2B6D2B27343}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Planning" sheetId="2" r:id="rId2"/>
     <sheet name="Testing-Results" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="163">
   <si>
     <t>File ID</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>75% training (1000pts) and testing, Hi Res</t>
+  </si>
+  <si>
+    <t>9, 10</t>
+  </si>
+  <si>
+    <t>1 runs with dataset 9,_x000D_
+2 runs with dataset 10 (flipped classes)_x000D_
+2 runs with dataset 9,_x000D_
+2 runs with dataset 10 (flipped classes)</t>
   </si>
 </sst>
 </file>
@@ -675,7 +684,17 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FFFAFAFA"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFAFAFA"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -775,11 +794,6 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFAFAFA"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -816,44 +830,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{956D0844-B19E-4710-9DAC-05F73E246C19}" name="Table2" displayName="Table2" ref="A1:T48" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{956D0844-B19E-4710-9DAC-05F73E246C19}" name="Table2" displayName="Table2" ref="A1:T48" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <tableColumns count="20">
-    <tableColumn id="15" xr3:uid="{FDC793E9-6539-479B-BBE9-DA7F4342D985}" name="Topic" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{2298DA6A-63A1-4496-9149-069EF69C148A}" name="Training_x000a_File ID" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{D92B2307-1F7B-4F64-84B8-FBA0372863B7}" name="Testing_x000a_File ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{51D40E01-7F15-4D7E-8885-D4CF31978D32}" name="Result_x000a_ID" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{95BB7443-5C91-4124-9452-D0BB24533E54}" name="DataSet" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{E760823C-C26C-4A12-B930-A04436170C6F}" name="Description" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A80AC177-3117-4101-B886-3A6D1CE2C6B4}" name="Exp._x000a_Rate" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{1025810D-4F5C-4D7E-8D36-25D6AF31CA8F}" name="Disc._x000a_Factor" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{3850DDDD-55B8-4C2E-9B23-B791C588561E}" name="Parallel Query Updates" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{4AD059AD-7B22-49BE-A02A-142A95E88A7C}" name="Parallel Report Updates" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{68CBAC58-A286-4D6D-BF13-ACE68E0468DB}" name="Total_x000a_Passes" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{3B1F9CB1-142C-44DF-86D5-58E1838E08EA}" name="Correct_x000a_Count" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{3ADE0F5F-F276-452A-9472-8553E8282D3D}" name="Points_x000a_Checked" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{61CCADA9-8789-44BA-B6B7-BA04D3A82703}" name="Percent_x000a_Correct" dataDxfId="6">
+    <tableColumn id="15" xr3:uid="{FDC793E9-6539-479B-BBE9-DA7F4342D985}" name="Topic" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{2298DA6A-63A1-4496-9149-069EF69C148A}" name="Training_x000a_File ID" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{D92B2307-1F7B-4F64-84B8-FBA0372863B7}" name="Testing_x000a_File ID" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{51D40E01-7F15-4D7E-8885-D4CF31978D32}" name="Result_x000a_ID" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{95BB7443-5C91-4124-9452-D0BB24533E54}" name="DataSet" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{E760823C-C26C-4A12-B930-A04436170C6F}" name="Description" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{A80AC177-3117-4101-B886-3A6D1CE2C6B4}" name="Exp._x000a_Rate" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1025810D-4F5C-4D7E-8D36-25D6AF31CA8F}" name="Disc._x000a_Factor" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{3850DDDD-55B8-4C2E-9B23-B791C588561E}" name="Parallel Query Updates" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{4AD059AD-7B22-49BE-A02A-142A95E88A7C}" name="Parallel Report Updates" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{68CBAC58-A286-4D6D-BF13-ACE68E0468DB}" name="Total_x000a_Passes" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{3B1F9CB1-142C-44DF-86D5-58E1838E08EA}" name="Correct_x000a_Count" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{3ADE0F5F-F276-452A-9472-8553E8282D3D}" name="Points_x000a_Checked" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{61CCADA9-8789-44BA-B6B7-BA04D3A82703}" name="Percent_x000a_Correct" dataDxfId="8">
       <calculatedColumnFormula>Table2[[#This Row],[Correct
 Count]]/Table2[[#This Row],[Points
 Checked]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{7BED7778-28C8-491D-9B04-7FE61C0061A4}" name="Total_x000a_States" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{DB683034-F593-424C-BBAF-9B9560CDB331}" name="Processing Time (sec)" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{1FCE8FC3-76B3-4188-803B-C37FBC9A1E5C}" name="Details" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{7BED7778-28C8-491D-9B04-7FE61C0061A4}" name="Total_x000a_States" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{DB683034-F593-424C-BBAF-9B9560CDB331}" name="Processing Time (sec)" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{1FCE8FC3-76B3-4188-803B-C37FBC9A1E5C}" name="Details" dataDxfId="5">
       <calculatedColumnFormula>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-details.txt", "Details " &amp; Table2[[#This Row],[Result
 ID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B4CAD1FD-A822-4390-8AD5-AE11A7788443}" name="Tree" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{B4CAD1FD-A822-4390-8AD5-AE11A7788443}" name="Tree" dataDxfId="4">
       <calculatedColumnFormula>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-tree.png", "Tree " &amp; Table2[[#This Row],[Result
 ID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{153E0BAC-13D7-4D63-96FB-294A4D5C2D90}" name="Chart" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{153E0BAC-13D7-4D63-96FB-294A4D5C2D90}" name="Chart" dataDxfId="3">
       <calculatedColumnFormula>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-chart.png", "Chart " &amp; Table2[[#This Row],[Result
 ID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9C6E6FE5-B403-42C5-A0DA-F89AA4046D05}" name="Data" dataDxfId="0">
+    <tableColumn id="13" xr3:uid="{9C6E6FE5-B403-42C5-A0DA-F89AA4046D05}" name="Data" dataDxfId="2">
       <calculatedColumnFormula>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;".csv", "Open CSV " &amp; Table2[[#This Row],[Result
 ID]])</calculatedColumnFormula>
@@ -1163,8 +1177,8 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1841,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C74B03-593C-453D-A782-F225B3E217F0}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5401,64 +5415,81 @@
         <v>Open CSV 46</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:20" ht="57" x14ac:dyDescent="0.45">
       <c r="A48" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" s="3">
+        <v>47</v>
+      </c>
       <c r="E48" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="7"/>
+      <c r="F48" s="17" t="s">
+        <v>162</v>
+      </c>
       <c r="G48" s="4">
         <v>0</v>
       </c>
       <c r="H48" s="5">
         <v>0.85</v>
       </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="8" t="e">
-        <f>Table2[[#This Row],[Correct
-Count]]/Table2[[#This Row],[Points
-Checked]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O48" s="9"/>
+      <c r="I48" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="18">
+        <v>7</v>
+      </c>
+      <c r="L48" s="13">
+        <v>8062</v>
+      </c>
+      <c r="M48" s="5">
+        <v>8124</v>
+      </c>
+      <c r="N48" s="8">
+        <v>99.2</v>
+      </c>
+      <c r="O48" s="9">
+        <v>4465</v>
+      </c>
       <c r="P48" s="23"/>
       <c r="Q48" s="6" t="str">
         <f>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-details.txt", "Details " &amp; Table2[[#This Row],[Result
 ID]])</f>
-        <v xml:space="preserve">Details </v>
+        <v>Details 47</v>
       </c>
       <c r="R48" s="6" t="str">
         <f>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-tree.png", "Tree " &amp; Table2[[#This Row],[Result
 ID]])</f>
-        <v xml:space="preserve">Tree </v>
+        <v>Tree 47</v>
       </c>
       <c r="S48" s="6" t="str">
         <f>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;"-chart.png", "Chart " &amp; Table2[[#This Row],[Result
 ID]])</f>
-        <v xml:space="preserve">Chart </v>
+        <v>Chart 47</v>
       </c>
       <c r="T48" s="6" t="str">
         <f>HYPERLINK("Results\"&amp;Table2[[#This Row],[Result
 ID]]&amp;".csv", "Open CSV " &amp; Table2[[#This Row],[Result
 ID]])</f>
-        <v xml:space="preserve">Open CSV </v>
+        <v>Open CSV 47</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q2:T48">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>ISBLANK($D2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>